<commit_message>
Lets go Possible Update
Lets go Mega Page
Updated Mega Starmie from Phoenix to Mega Starmie H
Updated Task List
</commit_message>
<xml_diff>
--- a/Data Input Sheets/Task List.xlsx
+++ b/Data Input Sheets/Task List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mango\OneDrive\Documents\GitHub\pokemon_game\Data Input Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="26A3C0098BED397DE4AF5129F67D6ACBB6CC251C" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{C597F521-8CEA-477B-BB71-3A3B1EA15700}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="26A3C0098BED397DE4AF5129F67D6ACBB6CC251C" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{4D60F478-1B3F-4FB0-B927-19CA4EA69E63}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" xr2:uid="{0A7390FF-04FC-4544-8468-1EF828D14CD2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="118">
   <si>
     <t>Comments</t>
   </si>
@@ -364,6 +364,21 @@
   </si>
   <si>
     <t>Double Up Downloaded Icons</t>
+  </si>
+  <si>
+    <t>New Tasks/Projects</t>
+  </si>
+  <si>
+    <t>Sage 2.0</t>
+  </si>
+  <si>
+    <t>Phoenix Rising</t>
+  </si>
+  <si>
+    <t>Lets Go?</t>
+  </si>
+  <si>
+    <t>See Short Term List</t>
   </si>
 </sst>
 </file>
@@ -725,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E390785-516B-41F9-B907-09498673F001}">
-  <dimension ref="A1:O38"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1243,6 +1258,31 @@
         <v>99</v>
       </c>
     </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>117</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>